<commit_message>
All testing done + most TODOs
</commit_message>
<xml_diff>
--- a/theses/Odpovedi.xlsx
+++ b/theses/Odpovedi.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\Michaela\Skola\VS\bakalarka\python\pymupdf\Theses-Checker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\Michaela\Skola\VS\bakalarka\python\pymupdf\Theses-Checker\theses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9228ED06-3659-464B-B9BC-0DA1547C6EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277069CD-AC7F-4173-9AB8-4D09055AC597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{466126B8-30B6-459D-8490-4F2EBCF8186B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{466126B8-30B6-459D-8490-4F2EBCF8186B}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
-    <sheet name="List2" sheetId="2" r:id="rId2"/>
-    <sheet name="List2 (2)" sheetId="4" r:id="rId3"/>
-    <sheet name="List2 (3)" sheetId="5" r:id="rId4"/>
-    <sheet name="List2 (4)" sheetId="6" r:id="rId5"/>
-    <sheet name="List2 (5)" sheetId="7" r:id="rId6"/>
-    <sheet name="List2 (6)" sheetId="8" r:id="rId7"/>
-    <sheet name="List2 (7)" sheetId="9" r:id="rId8"/>
+    <sheet name="hodnoceni oznaceni" sheetId="2" r:id="rId2"/>
+    <sheet name="dokázali jste zkontrolovat" sheetId="4" r:id="rId3"/>
+    <sheet name="dokázali jste nahrát" sheetId="5" r:id="rId4"/>
+    <sheet name="pop-up anotace" sheetId="6" r:id="rId5"/>
+    <sheet name="špatné označení" sheetId="7" r:id="rId6"/>
+    <sheet name="práce se stránkou jednoduchá" sheetId="8" r:id="rId7"/>
+    <sheet name="prohlížeč" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="72">
   <si>
     <t>Časová značka</t>
   </si>
@@ -251,6 +250,36 @@
   <si>
     <t>Safari</t>
   </si>
+  <si>
+    <t>Špatně uvedená reference</t>
+  </si>
+  <si>
+    <t>Dej do predchozi otazky moznost ostatni. 
+Nachazelo mi to pomlcky v lstlisting (kodu). Coz mi navadilo, ale nevidel bych to za chybu.</t>
+  </si>
+  <si>
+    <t>Nemusel bych to tam nahravat 2x :D</t>
+  </si>
+  <si>
+    <t>hlidani footnote, priklad: Flutter 6 -&gt; aby to bylo Flutter\footnote{.....
+naopak hlidani mezer u \ref{} aby to nebylo kapitola5.7 -&gt; ale kapitola \ref{.....
+Ale je to pecka!</t>
+  </si>
+  <si>
+    <t>bylo označeno za chybu "help()", ale help je název funkce, bylo označeno za chybu "P[x]", ale jedná se o součýst rovnice</t>
+  </si>
+  <si>
+    <t>Niektoré anotácie nezobrazili pop-up a nevedel som, čo s nimi bolo zle: napríklad mám figure na celú šírku stránky a checker mi na jej ľavý a pravý okraj pridal červené čiary s nejakými šípkami. Netuším ale, čo chcel povedať</t>
+  </si>
+  <si>
+    <t>Vynechaná mezera před levou závorkou, Výskyt textu mezi nadpisy, Oznacenie dolneho indexu ako zatvorky, ktorej chyba medzera na lavej strane</t>
+  </si>
+  <si>
+    <t>Oznacovanie chybajucej medzery pred zatvorkou v matematickych funkciach v matematickom prostredi, napr `sin(x)`.</t>
+  </si>
+  <si>
+    <t>vynechaná medzera pred zatvorkou v názvoch funkcií bola označena za chybu ako aj pred zatvrkou v rovniciach ale to je mozno ok</t>
+  </si>
 </sst>
 </file>
 
@@ -290,7 +319,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -333,6 +362,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -348,11 +388,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,8 +451,41 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E483251B-D855-4A8C-9B1D-3621280A0937}" type="CELLRANGE">
+                    <a:fld id="{81A9C0AA-6533-4CFB-8C4B-8866BCD087B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[OBLAST BUNĚK]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="cs-CZ"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-FA7D-4AF4-AD2F-440C68D0C15F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A7227834-32D8-4349-B347-9FC6FBA37C38}" type="CELLRANGE">
+                      <a:rPr lang="cs-CZ"/>
                       <a:pPr/>
                       <a:t>[OBLAST BUNĚK]</a:t>
                     </a:fld>
@@ -430,26 +507,23 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-FA7D-4AF4-AD2F-440C68D0C15F}"/>
+                  <c16:uniqueId val="{00000003-FA7D-4AF4-AD2F-440C68D0C15F}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="1"/>
+              <c:idx val="2"/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73062DC7-E4C8-4D21-8EEE-095949184BAE}" type="VALUE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{10F2A8E7-1961-493B-8F1F-C81C694234AA}" type="CELLRANGE">
+                      <a:rPr lang="cs-CZ"/>
                       <a:pPr/>
-                      <a:t>[HODNOTA]</a:t>
+                      <a:t>[OBLAST BUNĚK]</a:t>
                     </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t> (0 %)</a:t>
-                    </a:r>
+                    <a:endParaRPr lang="cs-CZ"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -463,36 +537,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-FA7D-4AF4-AD2F-440C68D0C15F}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>2 (7,7 %)</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -507,15 +552,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4053145-F617-4AFD-BFD2-5DD547E0E713}" type="VALUE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{82F0EF85-C2C5-4039-8CB4-5FAEBD45ADC2}" type="CELLRANGE">
+                      <a:rPr lang="cs-CZ"/>
                       <a:pPr/>
-                      <a:t>[HODNOTA]</a:t>
+                      <a:t>[OBLAST BUNĚK]</a:t>
                     </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t> (38,5 %)</a:t>
-                    </a:r>
+                    <a:endParaRPr lang="cs-CZ"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -529,6 +571,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -543,15 +586,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86675ECC-F429-4586-B015-3C00BD95EC88}" type="VALUE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{3B95497C-9332-48B4-B3AF-9CF347E7C91A}" type="CELLRANGE">
+                      <a:rPr lang="cs-CZ"/>
                       <a:pPr/>
-                      <a:t>[HODNOTA]</a:t>
+                      <a:t>[OBLAST BUNĚK]</a:t>
                     </a:fld>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t> (53,8 %)</a:t>
-                    </a:r>
+                    <a:endParaRPr lang="cs-CZ"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -565,6 +605,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -573,9 +614,7 @@
               </c:extLst>
             </c:dLbl>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -592,7 +631,7 @@
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showDataLabelsRange val="1"/>
-                <c15:showLeaderLines val="0"/>
+                <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -601,11 +640,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>List2!$L$5:$L$10</c15:sqref>
+                    <c15:sqref>'hodnoceni oznaceni'!$L$5:$L$10</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>List2!$L$5:$L$9</c:f>
+              <c:f>'hodnoceni oznaceni'!$L$5:$L$9</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -631,11 +670,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>List2!$M$5:$M$10</c15:sqref>
+                    <c15:sqref>'hodnoceni oznaceni'!$M$5:$M$10</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>List2!$M$5:$M$9</c:f>
+              <c:f>'hodnoceni oznaceni'!$M$5:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -646,13 +685,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -660,9 +699,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>List2!$O$5:$O$9</c15:f>
+                <c15:f>'hodnoceni oznaceni'!$O$5:$O$10</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="6"/>
                   <c:pt idx="0">
                     <c:v>0 (0 %)</c:v>
                   </c:pt>
@@ -670,13 +709,16 @@
                     <c:v>0 (0 %)</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2 (7,7 %)</c:v>
+                    <c:v>3 (8,8 %)</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>10 (38,5 %)</c:v>
+                    <c:v>11 (32,4 %)</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>14 (53,8 %)</c:v>
+                    <c:v>20 (58,8 %)</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0 (0 %)</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -706,6 +748,27 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ" sz="1200">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Hodnocení</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -746,6 +809,35 @@
             </a:ln>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ" sz="1200">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Počet odpovědí</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.3051006828656722E-2"/>
+              <c:y val="0.20356712765642665"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -771,6 +863,11 @@
     </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -833,7 +930,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'List2 (2)'!$E$3</c:f>
+              <c:f>'dokázali jste zkontrolovat'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -856,6 +953,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-92EB-4B8A-878F-F77E2801BB65}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -871,10 +973,15 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-92EB-4B8A-878F-F77E2801BB65}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'List2 (2)'!$D$4:$D$5</c:f>
+              <c:f>'dokázali jste zkontrolovat'!$D$4:$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -888,12 +995,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'List2 (2)'!$E$4:$E$5</c:f>
+              <c:f>'dokázali jste zkontrolovat'!$E$4:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1048,7 +1155,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'List2 (3)'!$E$3</c:f>
+              <c:f>'dokázali jste nahrát'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1099,7 +1206,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'List2 (3)'!$D$4:$D$5</c:f>
+              <c:f>'dokázali jste nahrát'!$D$4:$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1113,12 +1220,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'List2 (3)'!$E$4:$E$5</c:f>
+              <c:f>'dokázali jste nahrát'!$E$4:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1273,7 +1380,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'List2 (4)'!$E$3</c:f>
+              <c:f>'pop-up anotace'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1324,7 +1431,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'List2 (4)'!$D$4:$D$5</c:f>
+              <c:f>'pop-up anotace'!$D$4:$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1338,15 +1445,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'List2 (4)'!$E$4:$E$5</c:f>
+              <c:f>'pop-up anotace'!$E$4:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1458,37 +1565,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="cs-CZ"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -1498,7 +1575,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'List2 (5)'!$E$3</c:f>
+              <c:f>'špatné označení'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1514,10 +1591,8 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1535,9 +1610,7 @@
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1547,9 +1620,156 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{28659106-7CA5-4CAF-A98F-03B16A5D744C}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[HODNOTA]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (</a:t>
+                    </a:r>
+                    <a:fld id="{389A8E9B-08C1-44BF-A878-0ED231C2E258}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PROCENTO]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator> (</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-51B6-4A8B-A495-FDB588874610}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{8C2276F3-F0AD-423B-9AF1-2F8B90B53602}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[HODNOTA]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (</a:t>
+                    </a:r>
+                    <a:fld id="{6CAB6AFE-F982-4D51-A500-945CA0053E44}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PROCENTO]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator> (</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-51B6-4A8B-A495-FDB588874610}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="cs-CZ"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:separator> (</c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'List2 (5)'!$D$4:$D$5</c:f>
+              <c:f>'špatné označení'!$D$4:$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1563,15 +1783,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'List2 (5)'!$E$4:$E$5</c:f>
+              <c:f>'špatné označení'!$E$4:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1584,7 +1804,7 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1602,21 +1822,23 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:softEdge rad="0"/>
+        </a:effectLst>
       </c:spPr>
       <c:txPr>
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1641,12 +1863,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1723,7 +1940,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'List2 (6)'!$E$3</c:f>
+              <c:f>'práce se stránkou jednoduchá'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1774,7 +1991,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'List2 (6)'!$D$4:$D$5</c:f>
+              <c:f>'práce se stránkou jednoduchá'!$D$4:$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1788,12 +2005,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'List2 (6)'!$E$4:$E$5</c:f>
+              <c:f>'práce se stránkou jednoduchá'!$E$4:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1908,39 +2125,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="cs-CZ"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22240681014169747"/>
+          <c:y val="0.1520364970502307"/>
+          <c:w val="0.45336210819344658"/>
+          <c:h val="0.77650985324474631"/>
+        </c:manualLayout>
+      </c:layout>
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -1948,7 +2145,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'List2 (7)'!$E$3</c:f>
+              <c:f>prohlížeč!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2079,22 +2276,120 @@
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="1"/>
+              <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.5163092282063513E-2"/>
-                  <c:y val="5.4791309465558151E-2"/>
+                  <c:x val="-4.1820414660113527E-2"/>
+                  <c:y val="0.12535109587032295"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2A2BA478-8A8F-45FC-9363-E1D0DA8A0F94}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[NÁZEV KATEGORIE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{F84650E8-F37B-4297-BAAA-E4F7AC657A18}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[HODNOTA]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (</a:t>
+                    </a:r>
+                    <a:fld id="{030A18B3-FB75-408E-AD33-34B918F56E01}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PROCENTO]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showLegendKey val="1"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-DCA8-455B-B06D-BDA46CA57A03}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.7471202672389163E-4"/>
+                  <c:y val="6.8221875669761192E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DDBFC1A5-F08A-451E-AB4B-E2F1C3F6E751}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[NÁZEV KATEGORIE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{583B1CC8-6088-416D-92A8-4E42B0B0BC6D}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[HODNOTA]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (</a:t>
+                    </a:r>
+                    <a:fld id="{5030378A-353C-4E6C-8A58-69F0F18CB51E}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PROCENTO]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="1"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-DCA8-455B-B06D-BDA46CA57A03}"/>
                 </c:ext>
@@ -2104,19 +2399,59 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.957129399716051E-2"/>
-                  <c:y val="-0.12328044629750602"/>
+                  <c:x val="-1.0964069636753065E-2"/>
+                  <c:y val="6.9222992408432993E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C0521599-CA04-4F1D-8BE8-84A60C774F0F}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[NÁZEV KATEGORIE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>;</a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{FC9B507B-7D88-4E08-93A9-5EF8E5CADEB4}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[HODNOTA]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (</a:t>
+                    </a:r>
+                    <a:fld id="{4AA8DF4E-FE3D-4155-9C94-74B83CA37015}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PROCENTO]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showLegendKey val="1"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-DCA8-455B-B06D-BDA46CA57A03}"/>
                 </c:ext>
@@ -2126,19 +2461,57 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.3122083706578532E-2"/>
-                  <c:y val="8.6752906653800449E-2"/>
+                  <c:x val="-2.8181032178051239E-2"/>
+                  <c:y val="-8.7843411241836047E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E71EF290-3C54-4EA5-88C9-1AEE07CD7FE4}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[NÁZEV KATEGORIE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{86B14D4B-FE26-443B-80CC-C46F55EB32B4}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[HODNOTA]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (</a:t>
+                    </a:r>
+                    <a:fld id="{58F462C6-7ECB-482E-8BC5-FA8ECF9B9B4C}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PROCENTO]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showLegendKey val="1"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-DCA8-455B-B06D-BDA46CA57A03}"/>
                 </c:ext>
@@ -2148,21 +2521,127 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.7958991424515017E-3"/>
-                  <c:y val="-7.7621021742874163E-2"/>
+                  <c:x val="1.4889261311938514E-3"/>
+                  <c:y val="-5.971379341462589E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{506069EC-E78A-4273-909D-BAAD15AD8319}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[NÁZEV KATEGORIE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{E84053A3-945C-4F9F-9C82-4BE078EFA7A3}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[HODNOTA]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (</a:t>
+                    </a:r>
+                    <a:fld id="{39F64A8A-C58B-4133-9B58-8FEEA30A97C2}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PROCENTO]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
+              <c:showLegendKey val="1"/>
+              <c:showVal val="1"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.19161056138349836"/>
+                      <c:h val="0.1128780273206168"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-DCA8-455B-B06D-BDA46CA57A03}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8296431413799625E-2"/>
+                  <c:y val="-1.7907299410046127E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B416E17B-D56D-4045-8377-7E73C857A837}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[NÁZEV KATEGORIE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{38AD2709-EE47-4767-B1A0-95616598B291}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[HODNOTA]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> (</a:t>
+                    </a:r>
+                    <a:fld id="{FBAA2064-9395-4328-8B09-554671DE00CC}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[PROCENTO]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>)</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="1"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-DCA8-455B-B06D-BDA46CA57A03}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2203,8 +2682,8 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showLegendKey val="1"/>
+            <c:showVal val="1"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="1"/>
@@ -2226,7 +2705,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'List2 (7)'!$D$4:$D$9</c:f>
+              <c:f>prohlížeč!$D$4:$D$9</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2252,24 +2731,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'List2 (7)'!$E$4:$E$9</c:f>
+              <c:f>prohlížeč!$E$4:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3</c:v>
@@ -2342,12 +2821,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -5735,9 +6209,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>12390</xdr:rowOff>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5896,16 +6370,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>105833</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>10583</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>14816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>556591</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>145775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6318,9 +6792,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236582D1-CCC3-495C-8663-E9147CE4F0E9}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7232,115 +7706,265 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+    <row r="28" spans="1:12" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>45051.543449074074</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="3">
+        <v>5</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="L28" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="A29" s="2">
+        <v>45052.656597222223</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="L29" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>45053.004571759258</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="3">
+        <v>5</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="A31" s="2">
+        <v>45053.729386574072</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="3">
+        <v>3</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="J31" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-    </row>
-    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="L31" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>45053.739479166667</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="3">
+        <v>5</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="A33" s="2">
+        <v>45053.742384259262</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="3">
+        <v>5</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+    <row r="34" spans="1:12" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>45054.57372685185</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="3">
+        <v>5</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="A35" s="2">
+        <v>45055.511817129627</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="3">
+        <v>5</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
@@ -7354,8 +7978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6B590A-9C0A-4443-B6F6-FCA4BE736D50}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7397,10 +8021,10 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -7408,10 +8032,11 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5">
+        <f>COUNTIF(A:A,L5)</f>
         <v>0</v>
       </c>
       <c r="N5">
@@ -7427,10 +8052,11 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6">
         <v>2</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6">
+        <f>COUNTIF(A:A,L6)</f>
         <v>0</v>
       </c>
       <c r="N6">
@@ -7446,67 +8072,70 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7">
         <v>3</v>
       </c>
-      <c r="M7" s="5">
-        <v>2</v>
+      <c r="M7">
+        <f>COUNTIF(A:A,L7)</f>
+        <v>3</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>7.6923076923076925</v>
+        <v>8.8235294117647065</v>
       </c>
       <c r="O7" t="str">
         <f>_xlfn.CONCAT(M7, " (",ROUND( N7,1), " %)")</f>
-        <v>2 (7,7 %)</v>
+        <v>3 (8,8 %)</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8">
         <v>4</v>
       </c>
-      <c r="M8" s="5">
-        <v>10</v>
+      <c r="M8">
+        <f t="shared" ref="M8:M9" si="2">COUNTIF(A:A,L8)</f>
+        <v>11</v>
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>38.461538461538467</v>
+        <v>32.352941176470587</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" ref="O8:O10" si="2">_xlfn.CONCAT(M8, " (",ROUND( N8,1), " %)")</f>
-        <v>10 (38,5 %)</v>
+        <f t="shared" ref="O8:O10" si="3">_xlfn.CONCAT(M8, " (",ROUND( N8,1), " %)")</f>
+        <v>11 (32,4 %)</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9">
         <v>5</v>
       </c>
-      <c r="M9" s="5">
-        <v>14</v>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
-        <v>53.846153846153847</v>
+        <v>58.82352941176471</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="2"/>
-        <v>14 (53,8 %)</v>
+        <f t="shared" si="3"/>
+        <v>20 (58,8 %)</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="4">
         <v>0</v>
       </c>
       <c r="N10">
@@ -7514,7 +8143,7 @@
         <v>0</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0 (0 %)</v>
       </c>
     </row>
@@ -7604,28 +8233,44 @@
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
+      <c r="A28" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+      <c r="A29" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="A30" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+      <c r="A31" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
+      <c r="A33" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
+      <c r="A34" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="A35" s="3">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L5:L9">
@@ -7642,7 +8287,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7679,8 +8324,8 @@
         <v>12</v>
       </c>
       <c r="E4">
-        <f>COUNTIF(A2:A27,"Ano")</f>
-        <v>26</v>
+        <f>COUNTIF(A:A,"Ano")</f>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7691,7 +8336,7 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <f>COUNTIF(A2:A27,"Ne")</f>
+        <f>COUNTIF(A:A,"Ne")</f>
         <v>0</v>
       </c>
     </row>
@@ -7806,28 +8451,44 @@
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -7841,7 +8502,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7878,8 +8539,8 @@
         <v>12</v>
       </c>
       <c r="E4">
-        <f>COUNTIF(A2:A27,"Ano")</f>
-        <v>26</v>
+        <f>COUNTIF(A:A,"Ano")</f>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7890,7 +8551,7 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <f>COUNTIF(A2:A27,"Ne")</f>
+        <f>COUNTIF(A:A,"Ne")</f>
         <v>0</v>
       </c>
     </row>
@@ -8005,28 +8666,44 @@
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8040,7 +8717,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8077,8 +8754,8 @@
         <v>12</v>
       </c>
       <c r="E4">
-        <f>COUNTIF(A2:A27,"Ano")</f>
-        <v>26</v>
+        <f>COUNTIF(A:A,"Ano")</f>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8089,8 +8766,8 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <f>COUNTIF(A2:A27,"Ne")</f>
-        <v>0</v>
+        <f>COUNTIF(A:A,"Ne")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8204,28 +8881,44 @@
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8238,8 +8931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E456DEC1-FB1C-47CA-82BA-AD8C93AEC10B}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8247,7 +8940,7 @@
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -8276,8 +8969,8 @@
         <v>12</v>
       </c>
       <c r="E4">
-        <f>COUNTIF(A2:A27,"Ano")</f>
-        <v>16</v>
+        <f>COUNTIF(A:A,"Ano")</f>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8288,8 +8981,8 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <f>COUNTIF(A2:A27,"Ne")</f>
-        <v>10</v>
+        <f>COUNTIF(A:A,"Ne")</f>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8403,28 +9096,44 @@
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8438,7 +9147,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8475,8 +9184,8 @@
         <v>12</v>
       </c>
       <c r="E4">
-        <f>COUNTIF(A2:A27,"Ano")</f>
-        <v>26</v>
+        <f>COUNTIF(A:A,"Ano")</f>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8487,7 +9196,7 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <f>COUNTIF(A2:A27,"Ne")</f>
+        <f>COUNTIF(A:A,"Ne")</f>
         <v>0</v>
       </c>
     </row>
@@ -8602,28 +9311,44 @@
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8634,10 +9359,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9357F4-B73F-41EA-945F-B9F7B171EE1C}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8674,8 +9399,8 @@
         <v>11</v>
       </c>
       <c r="E4">
-        <f>COUNTIF($A$2:$A$27,"Google Chrome")</f>
-        <v>16</v>
+        <f>COUNTIF(A:A,"Google Chrome")</f>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8686,8 +9411,8 @@
         <v>15</v>
       </c>
       <c r="E5">
-        <f>COUNTIF(A2:A27,"Opera")</f>
-        <v>2</v>
+        <f>COUNTIF(A:A,"Opera")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8698,8 +9423,8 @@
         <v>61</v>
       </c>
       <c r="E6">
-        <f>COUNTIF(A2:A27,"Microsoft Edge")</f>
-        <v>0</v>
+        <f>COUNTIF(A:A,"Microsoft Edge")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8722,8 +9447,8 @@
         <v>28</v>
       </c>
       <c r="E8">
-        <f>COUNTIF(A2:A27,"Mozilla Firefox")</f>
-        <v>5</v>
+        <f>COUNTIF(A:A,"Mozilla Firefox")</f>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8734,7 +9459,7 @@
         <v>44</v>
       </c>
       <c r="E9">
-        <f>COUNTIF($A$2:$A$27,"Brave")</f>
+        <f>COUNTIF(A:A,"Brave")</f>
         <v>3</v>
       </c>
     </row>
@@ -8746,7 +9471,7 @@
         <v>56</v>
       </c>
       <c r="E10">
-        <f>COUNTA(A2:A27)-SUM(E4:E9)</f>
+        <f>COUNTA(A2:A99)-SUM(E4:E9)</f>
         <v>0</v>
       </c>
     </row>
@@ -8836,28 +9561,47 @@
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>